<commit_message>
extent report, tablet ready test scripts
extent report, tablet ready test scripts
</commit_message>
<xml_diff>
--- a/Appium_Capstone_Project/src/test/java/utils/credentials.xlsx
+++ b/Appium_Capstone_Project/src/test/java/utils/credentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collabera/eclipse-workspace/Appium_Capstone_Project/src/test/java/utils/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collabera/Documents/AppiumCapstone/Appium_Capstone_Project/src/test/java/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD26206-2C8E-5345-B6C6-4A1C9561A82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFD23AE-60E1-294B-BF45-7AC4194278CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="9400" windowWidth="28040" windowHeight="17440" xr2:uid="{91D57222-90E9-9348-A284-D122668F69E3}"/>
+    <workbookView xWindow="2200" yWindow="1080" windowWidth="28040" windowHeight="17440" xr2:uid="{91D57222-90E9-9348-A284-D122668F69E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC964A-95D6-B54E-9870-BB4D6BE5F1B1}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,6 +524,11 @@
         <v>500</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="mailto:rostel@gmail.com" xr:uid="{76CCB49B-B6D0-194E-82A3-1C4FB0025050}"/>

</xml_diff>